<commit_message>
Refactor documentation structure, enhance domain queue, and add configuration support
</commit_message>
<xml_diff>
--- a/reports/master_tracker.xlsx
+++ b/reports/master_tracker.xlsx
@@ -32,7 +32,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -57,6 +57,12 @@
         <bgColor rgb="00FFC000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D9EAD3"/>
+        <bgColor rgb="00D9EAD3"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -70,7 +76,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -81,6 +87,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -517,7 +524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,6 +551,1434 @@
       <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Added At</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>aeb.ac.lk</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>agc.sci.sjp.ac.lk</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>alumni.iit.ac.lk</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>app.wyb.ac.lk</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>application.ucj.ac.lk</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>apply.sltc.ac.lk</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>applyfgs.sjp.ac.lk</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>apps.esn.ac.lk</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>apps.kln.ac.lk</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>aptreg.mrt.ac.lk</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>apttests.mrt.ac.lk</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>arts.cmb.ac.lk</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>asaihl.kln.ac.lk</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>asr.cs.sjp.ac.lk</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>astrsoc.cmb.ac.lk</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>aua.cmb.ac.lk</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>auayf.cmb.ac.lk</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>autodiscover.apply.sltc.ac.lk</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>autodiscover.cdr.sjp.ac.lk</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>autodiscover.ncas.ac.lk</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>autodiscover.student.sliate.ac.lk</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>b3.ucsc.cmb.ac.lk</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>backup.medicine.kln.ac.lk</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>bit.cmb.ac.lk</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>bms.ac.lk</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>bpu.ac.lk</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>ca.learn.ac.lk</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>cal.kln.ac.lk</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>cal2.kln.ac.lk</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>campusradio.cmb.ac.lk</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>career.sjp.ac.lk</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>ccis.cmb.ac.lk</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>cct.cmb.ac.lk</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>cct.med.cmb.ac.lk</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>cdr.sjp.ac.lk</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>cdu.kln.ac.lk</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>ce.pdn.ac.lk</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>cefaq.ce.pdn.ac.lk</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>cell.cmb.ac.lk</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>cgu.cmb.ac.lk</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>chemsoc.cmb.ac.lk</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>cict.esn.ac.lk</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>cits.sjp.ac.lk</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>ciuc.cmb.ac.lk</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>clc.iit.ac.lk</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>cloud.esn.ac.lk</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>cmb.ac.lk</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>esn.ac.lk</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>fr.ac.lk</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>gs.ac.lk</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>gwu.ac.lk</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>iit.ac.lk</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>kdu.ac.lk</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>kiu.ac.lk</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>kln.ac.lk</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>mrt.ac.lk</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>ns2.ac.lk</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>ns3.ac.lk</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>nsf.ac.lk</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>ntp.ac.lk</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>ocu.ac.lk</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>oem.ac.lk</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>ou.ac.lk</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>ps.ac.lk</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>repo.ac.lk</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>rjt.ac.lk</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>seu.ac.lk</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>sjp.ac.lk</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>uca.ac.lk</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>ucb.ac.lk</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>uck.ac.lk</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>ucr.ac.lk</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>ugc.ac.lk</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>uom.ac.lk</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>url.ac.lk</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>uwu.ac.lk</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>vau.ac.lk</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>vpa.ac.lk</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>www.ac.lk</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="4" t="inlineStr">
+        <is>
+          <t>ac.lk</t>
+        </is>
+      </c>
+      <c r="B81" s="4" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="C81" s="4" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="4" t="inlineStr">
+        <is>
+          <t>accontroller.projects.mrt.ac.lk</t>
+        </is>
+      </c>
+      <c r="B82" s="4" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="C82" s="4" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="4" t="inlineStr">
+        <is>
+          <t>aces.ce.pdn.ac.lk</t>
+        </is>
+      </c>
+      <c r="B83" s="4" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="C83" s="4" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="4" t="inlineStr">
+        <is>
+          <t>ad.kln.ac.lk</t>
+        </is>
+      </c>
+      <c r="B84" s="4" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="C84" s="4" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="4" t="inlineStr">
+        <is>
+          <t>administration.kln.ac.lk</t>
+        </is>
+      </c>
+      <c r="B85" s="4" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="C85" s="4" t="inlineStr">
+        <is>
+          <t>2026-01-18 21:59:57</t>
         </is>
       </c>
     </row>

</xml_diff>